<commit_message>
Load cells at xlsx worksheet ingest; handle skipping and/or blank rows; fixes #224
</commit_message>
<xml_diff>
--- a/tests/testthat/sheets/blanks.xlsx
+++ b/tests/testthat/sheets/blanks.xlsx
@@ -1,17 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26915"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jenny/rrr/readxl/tests/testthat/sheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="24800" windowHeight="16580" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24800" windowHeight="16580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="different_rows" sheetId="1" r:id="rId1"/>
+    <sheet name="same_row_first" sheetId="2" r:id="rId2"/>
+    <sheet name="same_row_middle" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>x</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -32,12 +42,18 @@
     <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -74,7 +90,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -397,17 +418,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,24 +436,88 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>